<commit_message>
AI change to DS
</commit_message>
<xml_diff>
--- a/econ.xlsx
+++ b/econ.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29100" windowHeight="14540"/>
+    <workbookView windowWidth="22700" windowHeight="14520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="23">
   <si>
     <t>subject</t>
   </si>
@@ -65,19 +65,37 @@
     <t>subjects/econ/2025/AS/qp-202505-economics-p21</t>
   </si>
   <si>
+    <t>1.html</t>
+  </si>
+  <si>
+    <t>2.html</t>
+  </si>
+  <si>
     <t>3.html</t>
   </si>
   <si>
+    <t>4.html</t>
+  </si>
+  <si>
+    <t>5.html</t>
+  </si>
+  <si>
+    <t>qp-202505-economics-p22</t>
+  </si>
+  <si>
+    <t>subjects/econ/2025/AS/qp-202505-economics-p22</t>
+  </si>
+  <si>
     <t>qp-202505-economics-p24</t>
   </si>
   <si>
     <t>subjects/econ/2025/AS/qp-202505-economics-p24</t>
   </si>
   <si>
-    <t>5.html</t>
-  </si>
-  <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>6.html</t>
   </si>
 </sst>
 </file>
@@ -1244,10 +1262,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="7"/>
@@ -1301,6 +1319,9 @@
       <c r="F2" t="s">
         <v>11</v>
       </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
@@ -1321,6 +1342,9 @@
       <c r="F3" t="s">
         <v>11</v>
       </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
@@ -1342,7 +1366,7 @@
         <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1356,13 +1380,16 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1376,76 +1403,302 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>2025</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>2025</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s">
         <v>13</v>
       </c>
-      <c r="E6">
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>2025</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>2025</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>2025</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>2025</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>2025</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13">
         <v>2</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>2025</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="1" t="s">
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B15">
         <v>2025</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C15" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="2">
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="2">
         <v>5</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="2" t="s">
+      <c r="F16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="3"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="3"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="1"/>
+      <c r="H16" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="2">
+        <v>6</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="3"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>